<commit_message>
fixed conferences in team df
</commit_message>
<xml_diff>
--- a/data/NCAA_Team_D1_Stats.xlsx
+++ b/data/NCAA_Team_D1_Stats.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohanpoddar/Desktop/Columbia University/EDAV/Final Project/NCAAMensBasketball/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3CD8C9-60F2-EE45-B90B-8051A881DA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C42A11C-0767-8A48-A1E2-02C16A96DFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="15000" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AI$351</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="562">
   <si>
     <t>Team</t>
   </si>
@@ -1719,21 +1722,6 @@
   </si>
   <si>
     <t>Big Ten</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>FL</t>
-  </si>
-  <si>
-    <t>OH</t>
-  </si>
-  <si>
-    <t>PA</t>
-  </si>
-  <si>
-    <t>NY</t>
   </si>
 </sst>
 </file>
@@ -2094,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17332,7 +17320,7 @@
         <v>402</v>
       </c>
       <c r="B143" t="s">
-        <v>562</v>
+        <v>547</v>
       </c>
       <c r="C143" s="3">
         <v>29</v>
@@ -19365,7 +19353,7 @@
         <v>183</v>
       </c>
       <c r="B162" t="s">
-        <v>563</v>
+        <v>542</v>
       </c>
       <c r="C162" s="3">
         <v>37</v>
@@ -19472,7 +19460,7 @@
         <v>79</v>
       </c>
       <c r="B163" t="s">
-        <v>564</v>
+        <v>533</v>
       </c>
       <c r="C163" s="3">
         <v>32</v>
@@ -27818,7 +27806,7 @@
         <v>440</v>
       </c>
       <c r="B241" t="s">
-        <v>565</v>
+        <v>545</v>
       </c>
       <c r="C241" s="3">
         <v>30</v>
@@ -28139,7 +28127,7 @@
         <v>266</v>
       </c>
       <c r="B244" t="s">
-        <v>562</v>
+        <v>547</v>
       </c>
       <c r="C244" s="3">
         <v>34</v>
@@ -31349,7 +31337,7 @@
         <v>275</v>
       </c>
       <c r="B274" t="s">
-        <v>566</v>
+        <v>546</v>
       </c>
       <c r="C274" s="3">
         <v>32</v>
@@ -39691,6 +39679,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AI351" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D351">
     <sortCondition ref="A1:A351"/>
   </sortState>

</xml_diff>